<commit_message>
changement 4h à 3.5h
</commit_message>
<xml_diff>
--- a/documentation/3_1_Modele_Journal-Theo-Pasquier.xlsx
+++ b/documentation/3_1_Modele_Journal-Theo-Pasquier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/theo_pasquier_studentfr_ch/Documents/3eme année/306/projet/306-G1-Piloter_un_robot_phidget_a_distance/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FADF248E-E1A7-40DD-A13D-C66ABF56365A}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7DF3038-D1B9-4AEA-80C6-BC78B5C4E01A}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1167,7 +1167,7 @@
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <pane ySplit="1" activePane="bottomLeft"/>
       <selection activeCell="D5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="C6" s="33"/>
       <c r="D6" s="7">
-        <v>3.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1267,7 +1267,7 @@
       </c>
       <c r="D11" s="9">
         <f>SUM(D6:D10)</f>
-        <v>4</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -1776,7 +1776,7 @@
       </c>
       <c r="D83" s="12">
         <f>D11+D18+D25+D32+D39+D46+D53+D60+D67+D74+D81</f>
-        <v>4</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>